<commit_message>
added smote balancing and stuff
</commit_message>
<xml_diff>
--- a/Model_Results/AdaBoostClassifier/Result_AdaBoostClassifier_local.xlsx
+++ b/Model_Results/AdaBoostClassifier/Result_AdaBoostClassifier_local.xlsx
@@ -472,21 +472,23 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>91.66666666666666</v>
+        <v>65.22210184182016</v>
       </c>
       <c r="C2" t="n">
-        <v>84.02777777777779</v>
+        <v>64.18251735683648</v>
       </c>
       <c r="D2" t="n">
-        <v>91.66666666666666</v>
+        <v>65.22210184182016</v>
       </c>
       <c r="E2" t="n">
-        <v>87.68115942028986</v>
+        <v>64.51749665215661</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6498316498316499</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
+        <v>0.7028552813122796</v>
+      </c>
+      <c r="G2" t="n">
+        <v>35.05518933006285</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>